<commit_message>
india-education-map first draft complete
refactored code
</commit_message>
<xml_diff>
--- a/content/posts/india-education-map/india_school_data.xlsx
+++ b/content/posts/india-education-map/india_school_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thatgurjot/Git Repos/thatgurjot/content/posts/india-education-map/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D92B1617-36B5-4248-B060-29FBA8943DE1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30391A33-872D-8D4E-9399-3CF606B6A3E2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38080" yWindow="1800" windowWidth="25600" windowHeight="18100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="180" yWindow="460" windowWidth="15420" windowHeight="17540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Management" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="181">
   <si>
     <t/>
   </si>
@@ -562,6 +562,15 @@
   </si>
   <si>
     <t>4to5</t>
+  </si>
+  <si>
+    <t>Cambridge International Education</t>
+  </si>
+  <si>
+    <t>CIE</t>
+  </si>
+  <si>
+    <t>https://www.cambridgeinternational.org/cambridge-international-in-india/</t>
   </si>
 </sst>
 </file>
@@ -655,6 +664,10 @@
     <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -664,10 +677,6 @@
     <xf numFmtId="17" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -988,8 +997,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="J53" sqref="J53"/>
+    <sheetView topLeftCell="M3" workbookViewId="0">
+      <selection activeCell="R33" sqref="R33:R40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1008,11 +1017,11 @@
       <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
     </row>
     <row r="2" spans="1:20">
       <c r="A2" t="s">
@@ -1021,16 +1030,16 @@
       <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="17" t="s">
+      <c r="D2" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="18"/>
+      <c r="E2" s="15"/>
     </row>
     <row r="3" spans="1:20">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="15" t="s">
         <v>0</v>
       </c>
       <c r="D3" t="s">
@@ -1112,7 +1121,7 @@
       <c r="K5">
         <v>45</v>
       </c>
-      <c r="L5" s="14" t="s">
+      <c r="L5" s="16" t="s">
         <v>115</v>
       </c>
       <c r="N5">
@@ -1165,7 +1174,7 @@
       <c r="K6">
         <v>140</v>
       </c>
-      <c r="L6" s="15"/>
+      <c r="L6" s="17"/>
       <c r="N6">
         <f t="shared" ref="N6:N40" si="0">D6+E6</f>
         <v>47359</v>
@@ -1175,7 +1184,7 @@
         <v>16262</v>
       </c>
       <c r="P6">
-        <f t="shared" ref="P6:P41" si="2">N6/O6</f>
+        <f>N6/O6</f>
         <v>2.9122494158160128</v>
       </c>
       <c r="R6" s="4" t="s">
@@ -1184,7 +1193,7 @@
       <c r="S6">
         <v>1.1391597899474868</v>
       </c>
-      <c r="T6" s="14" t="s">
+      <c r="T6" s="16" t="s">
         <v>175</v>
       </c>
     </row>
@@ -1219,7 +1228,7 @@
       <c r="K7">
         <v>229</v>
       </c>
-      <c r="L7" s="15"/>
+      <c r="L7" s="17"/>
       <c r="N7">
         <f t="shared" si="0"/>
         <v>3243</v>
@@ -1229,7 +1238,7 @@
         <v>550</v>
       </c>
       <c r="P7">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="P6:P41" si="2">N7/O7</f>
         <v>5.8963636363636365</v>
       </c>
       <c r="R7" s="4" t="s">
@@ -1238,7 +1247,7 @@
       <c r="S7">
         <v>1.2673267326732673</v>
       </c>
-      <c r="T7" s="14"/>
+      <c r="T7" s="16"/>
     </row>
     <row r="8" spans="1:20">
       <c r="A8">
@@ -1271,7 +1280,7 @@
       <c r="K8">
         <v>346</v>
       </c>
-      <c r="L8" s="15"/>
+      <c r="L8" s="17"/>
       <c r="N8">
         <f t="shared" si="0"/>
         <v>52288</v>
@@ -1290,7 +1299,7 @@
       <c r="S8">
         <v>1.6113074204946995</v>
       </c>
-      <c r="T8" s="14"/>
+      <c r="T8" s="16"/>
     </row>
     <row r="9" spans="1:20">
       <c r="A9">
@@ -1323,7 +1332,7 @@
       <c r="K9">
         <v>414</v>
       </c>
-      <c r="L9" s="15"/>
+      <c r="L9" s="17"/>
       <c r="N9">
         <f t="shared" si="0"/>
         <v>73328</v>
@@ -1342,7 +1351,7 @@
       <c r="S9">
         <v>1.6172153024911031</v>
       </c>
-      <c r="T9" s="14"/>
+      <c r="T9" s="16"/>
     </row>
     <row r="10" spans="1:20">
       <c r="A10">
@@ -1375,7 +1384,7 @@
       <c r="K10">
         <v>739</v>
       </c>
-      <c r="L10" s="15"/>
+      <c r="L10" s="17"/>
       <c r="N10">
         <f t="shared" si="0"/>
         <v>128</v>
@@ -1394,7 +1403,7 @@
       <c r="S10">
         <v>1.6786957246355498</v>
       </c>
-      <c r="T10" s="14"/>
+      <c r="T10" s="16"/>
     </row>
     <row r="11" spans="1:20">
       <c r="A11">
@@ -1427,7 +1436,7 @@
       <c r="K11">
         <v>1290</v>
       </c>
-      <c r="L11" s="16" t="s">
+      <c r="L11" s="18" t="s">
         <v>116</v>
       </c>
       <c r="N11">
@@ -1448,7 +1457,7 @@
       <c r="S11">
         <v>1.7663026439544363</v>
       </c>
-      <c r="T11" s="14"/>
+      <c r="T11" s="16"/>
     </row>
     <row r="12" spans="1:20">
       <c r="A12">
@@ -1481,7 +1490,7 @@
       <c r="K12">
         <v>1486</v>
       </c>
-      <c r="L12" s="16"/>
+      <c r="L12" s="18"/>
       <c r="N12">
         <f t="shared" si="0"/>
         <v>310</v>
@@ -1500,7 +1509,7 @@
       <c r="S12">
         <v>2.093525179856115</v>
       </c>
-      <c r="T12" s="14" t="s">
+      <c r="T12" s="16" t="s">
         <v>176</v>
       </c>
     </row>
@@ -1535,7 +1544,7 @@
       <c r="K13">
         <v>2752</v>
       </c>
-      <c r="L13" s="16"/>
+      <c r="L13" s="18"/>
       <c r="N13">
         <f t="shared" si="0"/>
         <v>116</v>
@@ -1554,7 +1563,7 @@
       <c r="S13">
         <v>2.2634757834757835</v>
       </c>
-      <c r="T13" s="15"/>
+      <c r="T13" s="17"/>
     </row>
     <row r="14" spans="1:20">
       <c r="A14">
@@ -1587,7 +1596,7 @@
       <c r="K14">
         <v>3793</v>
       </c>
-      <c r="L14" s="16"/>
+      <c r="L14" s="18"/>
       <c r="N14">
         <f t="shared" si="0"/>
         <v>3037</v>
@@ -1606,7 +1615,7 @@
       <c r="S14">
         <v>2.5</v>
       </c>
-      <c r="T14" s="15"/>
+      <c r="T14" s="17"/>
     </row>
     <row r="15" spans="1:20">
       <c r="A15">
@@ -1639,7 +1648,7 @@
       <c r="K15">
         <v>3913</v>
       </c>
-      <c r="L15" s="16"/>
+      <c r="L15" s="18"/>
       <c r="N15">
         <f t="shared" si="0"/>
         <v>1347</v>
@@ -1658,7 +1667,7 @@
       <c r="S15">
         <v>2.5815153052595976</v>
       </c>
-      <c r="T15" s="15"/>
+      <c r="T15" s="17"/>
     </row>
     <row r="16" spans="1:20">
       <c r="A16">
@@ -1691,7 +1700,7 @@
       <c r="K16">
         <v>4844</v>
       </c>
-      <c r="L16" s="16"/>
+      <c r="L16" s="18"/>
       <c r="N16">
         <f t="shared" si="0"/>
         <v>40936</v>
@@ -1710,7 +1719,7 @@
       <c r="S16">
         <v>2.6939597315436243</v>
       </c>
-      <c r="T16" s="15"/>
+      <c r="T16" s="17"/>
     </row>
     <row r="17" spans="1:20">
       <c r="A17">
@@ -1743,7 +1752,7 @@
       <c r="K17">
         <v>4945</v>
       </c>
-      <c r="L17" s="16"/>
+      <c r="L17" s="18"/>
       <c r="N17">
         <f t="shared" si="0"/>
         <v>14542</v>
@@ -1762,7 +1771,7 @@
       <c r="S17">
         <v>2.7154616240266964</v>
       </c>
-      <c r="T17" s="15"/>
+      <c r="T17" s="17"/>
     </row>
     <row r="18" spans="1:20">
       <c r="A18">
@@ -1795,7 +1804,7 @@
       <c r="K18">
         <v>5703</v>
       </c>
-      <c r="L18" s="16"/>
+      <c r="L18" s="18"/>
       <c r="N18">
         <f t="shared" si="0"/>
         <v>15433</v>
@@ -1814,7 +1823,7 @@
       <c r="S18">
         <v>2.7918282279953472</v>
       </c>
-      <c r="T18" s="15"/>
+      <c r="T18" s="17"/>
     </row>
     <row r="19" spans="1:20">
       <c r="A19">
@@ -1847,7 +1856,7 @@
       <c r="K19">
         <v>14669</v>
       </c>
-      <c r="L19" s="14" t="s">
+      <c r="L19" s="16" t="s">
         <v>117</v>
       </c>
       <c r="N19">
@@ -1868,7 +1877,7 @@
       <c r="S19">
         <v>2.9122494158160128</v>
       </c>
-      <c r="T19" s="15"/>
+      <c r="T19" s="17"/>
     </row>
     <row r="20" spans="1:20">
       <c r="A20">
@@ -1901,7 +1910,7 @@
       <c r="K20">
         <v>16701</v>
       </c>
-      <c r="L20" s="14"/>
+      <c r="L20" s="16"/>
       <c r="N20">
         <f t="shared" si="0"/>
         <v>37131</v>
@@ -1920,7 +1929,7 @@
       <c r="S20">
         <v>2.9206190713929105</v>
       </c>
-      <c r="T20" s="15"/>
+      <c r="T20" s="17"/>
     </row>
     <row r="21" spans="1:20">
       <c r="A21">
@@ -1953,7 +1962,7 @@
       <c r="K21">
         <v>18212</v>
       </c>
-      <c r="L21" s="14"/>
+      <c r="L21" s="16"/>
       <c r="N21">
         <f t="shared" si="0"/>
         <v>57601</v>
@@ -1972,7 +1981,7 @@
       <c r="S21">
         <v>3.0000732869182851</v>
       </c>
-      <c r="T21" s="15"/>
+      <c r="T21" s="17"/>
     </row>
     <row r="22" spans="1:20">
       <c r="A22">
@@ -2005,7 +2014,7 @@
       <c r="K22">
         <v>23534</v>
       </c>
-      <c r="L22" s="14"/>
+      <c r="L22" s="16"/>
       <c r="N22">
         <f t="shared" si="0"/>
         <v>12206</v>
@@ -2024,7 +2033,7 @@
       <c r="S22">
         <v>3.0912162162162162</v>
       </c>
-      <c r="T22" s="15"/>
+      <c r="T22" s="17"/>
     </row>
     <row r="23" spans="1:20">
       <c r="A23">
@@ -2057,7 +2066,7 @@
       <c r="K23">
         <v>23559</v>
       </c>
-      <c r="L23" s="14"/>
+      <c r="L23" s="16"/>
       <c r="N23">
         <f t="shared" si="0"/>
         <v>45</v>
@@ -2075,7 +2084,7 @@
       <c r="S23">
         <v>3.5261305379141481</v>
       </c>
-      <c r="T23" s="15"/>
+      <c r="T23" s="17"/>
     </row>
     <row r="24" spans="1:20">
       <c r="A24">
@@ -2108,7 +2117,7 @@
       <c r="K24">
         <v>29708</v>
       </c>
-      <c r="L24" s="14"/>
+      <c r="L24" s="16"/>
       <c r="N24">
         <f t="shared" si="0"/>
         <v>122930</v>
@@ -2127,7 +2136,7 @@
       <c r="S24">
         <v>3.7252778569392988</v>
       </c>
-      <c r="T24" s="15"/>
+      <c r="T24" s="17"/>
     </row>
     <row r="25" spans="1:20">
       <c r="A25">
@@ -2160,7 +2169,7 @@
       <c r="K25">
         <v>42355</v>
       </c>
-      <c r="L25" s="14"/>
+      <c r="L25" s="16"/>
       <c r="N25">
         <f t="shared" si="0"/>
         <v>89587</v>
@@ -2179,7 +2188,7 @@
       <c r="S25">
         <v>3.948416522130147</v>
       </c>
-      <c r="T25" s="15"/>
+      <c r="T25" s="17"/>
     </row>
     <row r="26" spans="1:20">
       <c r="A26">
@@ -2212,7 +2221,7 @@
       <c r="K26">
         <v>45908</v>
       </c>
-      <c r="L26" s="14"/>
+      <c r="L26" s="16"/>
       <c r="N26">
         <f t="shared" si="0"/>
         <v>3660</v>
@@ -2231,7 +2240,7 @@
       <c r="S26">
         <v>4.2304887774866131</v>
       </c>
-      <c r="T26" s="14" t="s">
+      <c r="T26" s="16" t="s">
         <v>177</v>
       </c>
     </row>
@@ -2266,7 +2275,7 @@
       <c r="K27">
         <v>54581</v>
       </c>
-      <c r="L27" s="14" t="s">
+      <c r="L27" s="16" t="s">
         <v>118</v>
       </c>
       <c r="N27">
@@ -2287,7 +2296,7 @@
       <c r="S27">
         <v>4.3059474906233257</v>
       </c>
-      <c r="T27" s="15"/>
+      <c r="T27" s="17"/>
     </row>
     <row r="28" spans="1:20">
       <c r="A28">
@@ -2320,7 +2329,7 @@
       <c r="K28">
         <v>56274</v>
       </c>
-      <c r="L28" s="14"/>
+      <c r="L28" s="16"/>
       <c r="N28">
         <f t="shared" si="0"/>
         <v>2795</v>
@@ -2339,7 +2348,7 @@
       <c r="S28">
         <v>4.4012281994595925</v>
       </c>
-      <c r="T28" s="15"/>
+      <c r="T28" s="17"/>
     </row>
     <row r="29" spans="1:20">
       <c r="A29">
@@ -2372,7 +2381,7 @@
       <c r="K29">
         <v>59152</v>
       </c>
-      <c r="L29" s="14"/>
+      <c r="L29" s="16"/>
       <c r="N29">
         <f t="shared" si="0"/>
         <v>2007</v>
@@ -2391,7 +2400,7 @@
       <c r="S29">
         <v>4.4612807148175726</v>
       </c>
-      <c r="T29" s="15"/>
+      <c r="T29" s="17"/>
     </row>
     <row r="30" spans="1:20">
       <c r="A30">
@@ -2424,7 +2433,7 @@
       <c r="K30">
         <v>63621</v>
       </c>
-      <c r="L30" s="14"/>
+      <c r="L30" s="16"/>
       <c r="N30">
         <f t="shared" si="0"/>
         <v>61253</v>
@@ -2443,7 +2452,7 @@
       <c r="S30">
         <v>4.6129843985908403</v>
       </c>
-      <c r="T30" s="15"/>
+      <c r="T30" s="17"/>
     </row>
     <row r="31" spans="1:20">
       <c r="A31">
@@ -2476,7 +2485,7 @@
       <c r="K31">
         <v>66324</v>
       </c>
-      <c r="L31" s="14"/>
+      <c r="L31" s="16"/>
       <c r="N31">
         <f t="shared" si="0"/>
         <v>456</v>
@@ -2495,7 +2504,7 @@
       <c r="S31">
         <v>4.6712328767123283</v>
       </c>
-      <c r="T31" s="15"/>
+      <c r="T31" s="17"/>
     </row>
     <row r="32" spans="1:20">
       <c r="A32">
@@ -2528,7 +2537,7 @@
       <c r="K32">
         <v>68717</v>
       </c>
-      <c r="L32" s="14"/>
+      <c r="L32" s="16"/>
       <c r="N32">
         <f t="shared" si="0"/>
         <v>19862</v>
@@ -2547,7 +2556,7 @@
       <c r="S32">
         <v>4.833333333333333</v>
       </c>
-      <c r="T32" s="15"/>
+      <c r="T32" s="17"/>
     </row>
     <row r="33" spans="1:20">
       <c r="A33">
@@ -2580,7 +2589,7 @@
       <c r="K33">
         <v>78233</v>
       </c>
-      <c r="L33" s="14"/>
+      <c r="L33" s="16"/>
       <c r="N33">
         <f t="shared" si="0"/>
         <v>67607</v>
@@ -2599,7 +2608,7 @@
       <c r="S33">
         <v>5.5534364879453042</v>
       </c>
-      <c r="T33" s="14" t="s">
+      <c r="T33" s="16" t="s">
         <v>168</v>
       </c>
     </row>
@@ -2634,7 +2643,7 @@
       <c r="K34">
         <v>89224</v>
       </c>
-      <c r="L34" s="14"/>
+      <c r="L34" s="16"/>
       <c r="N34">
         <f t="shared" si="0"/>
         <v>873</v>
@@ -2653,7 +2662,7 @@
       <c r="S34">
         <v>5.5988532883642499</v>
       </c>
-      <c r="T34" s="15"/>
+      <c r="T34" s="17"/>
     </row>
     <row r="35" spans="1:20">
       <c r="A35">
@@ -2686,7 +2695,7 @@
       <c r="K35">
         <v>97828</v>
       </c>
-      <c r="L35" s="14"/>
+      <c r="L35" s="16"/>
       <c r="N35">
         <f t="shared" si="0"/>
         <v>46083</v>
@@ -2705,7 +2714,7 @@
       <c r="S35">
         <v>5.8963636363636365</v>
       </c>
-      <c r="T35" s="15"/>
+      <c r="T35" s="17"/>
     </row>
     <row r="36" spans="1:20">
       <c r="A36">
@@ -2738,7 +2747,7 @@
       <c r="K36">
         <v>105883</v>
       </c>
-      <c r="L36" s="14" t="s">
+      <c r="L36" s="16" t="s">
         <v>119</v>
       </c>
       <c r="N36">
@@ -2759,7 +2768,7 @@
       <c r="S36">
         <v>6.8496303529083553</v>
       </c>
-      <c r="T36" s="15"/>
+      <c r="T36" s="17"/>
     </row>
     <row r="37" spans="1:20">
       <c r="A37">
@@ -2792,7 +2801,7 @@
       <c r="K37">
         <v>109942</v>
       </c>
-      <c r="L37" s="14"/>
+      <c r="L37" s="16"/>
       <c r="N37">
         <f t="shared" si="0"/>
         <v>4355</v>
@@ -2811,7 +2820,7 @@
       <c r="S37">
         <v>7.3813559322033901</v>
       </c>
-      <c r="T37" s="15"/>
+      <c r="T37" s="17"/>
     </row>
     <row r="38" spans="1:20">
       <c r="A38">
@@ -2844,7 +2853,7 @@
       <c r="K38">
         <v>154064</v>
       </c>
-      <c r="L38" s="14"/>
+      <c r="L38" s="16"/>
       <c r="N38">
         <f t="shared" si="0"/>
         <v>171232</v>
@@ -2863,7 +2872,7 @@
       <c r="S38">
         <v>8.2064576634512321</v>
       </c>
-      <c r="T38" s="15"/>
+      <c r="T38" s="17"/>
     </row>
     <row r="39" spans="1:20">
       <c r="A39">
@@ -2896,7 +2905,7 @@
       <c r="K39">
         <v>273235</v>
       </c>
-      <c r="L39" s="14"/>
+      <c r="L39" s="16"/>
       <c r="N39">
         <f t="shared" si="0"/>
         <v>17550</v>
@@ -2915,7 +2924,7 @@
       <c r="S39">
         <v>8.6111111111111107</v>
       </c>
-      <c r="T39" s="15"/>
+      <c r="T39" s="17"/>
     </row>
     <row r="40" spans="1:20">
       <c r="A40">
@@ -2962,7 +2971,7 @@
       <c r="S40">
         <v>9.6906474820143877</v>
       </c>
-      <c r="T40" s="15"/>
+      <c r="T40" s="17"/>
     </row>
     <row r="41" spans="1:20">
       <c r="A41" t="s">
@@ -3459,11 +3468,6 @@
     </sortState>
   </autoFilter>
   <mergeCells count="12">
-    <mergeCell ref="D1:F1"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="L5:L10"/>
-    <mergeCell ref="T6:T11"/>
     <mergeCell ref="T12:T25"/>
     <mergeCell ref="T26:T32"/>
     <mergeCell ref="T33:T40"/>
@@ -3471,6 +3475,11 @@
     <mergeCell ref="L11:L18"/>
     <mergeCell ref="L27:L35"/>
     <mergeCell ref="L36:L39"/>
+    <mergeCell ref="D1:F1"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="L5:L10"/>
+    <mergeCell ref="T6:T11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3480,8 +3489,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DAF9762-A46F-424F-8185-B70B5BC484D4}">
   <dimension ref="A1:F53"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="E36" sqref="E36"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -3499,8 +3508,8 @@
       <c r="D1" s="19" t="s">
         <v>98</v>
       </c>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
@@ -3509,14 +3518,14 @@
       <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="17"/>
-      <c r="E2" s="18"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="15"/>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="15" t="s">
         <v>0</v>
       </c>
       <c r="D3" t="s">
@@ -3984,15 +3993,29 @@
     </row>
     <row r="44" spans="1:5">
       <c r="B44" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="D44">
+        <v>400</v>
+      </c>
+      <c r="E44" s="8" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="B45" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="C44" s="4" t="s">
+      <c r="C45" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="D44">
+      <c r="D45">
         <v>32000</v>
       </c>
-      <c r="E44" s="8" t="s">
+      <c r="E45" s="8" t="s">
         <v>112</v>
       </c>
     </row>
@@ -4006,21 +4029,21 @@
     </row>
     <row r="52" spans="2:5">
       <c r="D52">
-        <v>24084</v>
+        <v>106484</v>
       </c>
       <c r="E52">
         <f>D52*100/D51</f>
-        <v>1.5528046421663444</v>
+        <v>6.8655061250805929</v>
       </c>
     </row>
     <row r="53" spans="2:5">
       <c r="D53">
         <f>D51-D52</f>
-        <v>1526916</v>
+        <v>1444516</v>
       </c>
       <c r="E53" s="7">
         <f>D53*100/D51</f>
-        <v>98.44719535783365</v>
+        <v>93.1344938749194</v>
       </c>
     </row>
   </sheetData>
@@ -4033,7 +4056,8 @@
     <hyperlink ref="E41" r:id="rId1" xr:uid="{C276C17D-F950-BC48-863D-3160A30B472C}"/>
     <hyperlink ref="E42" r:id="rId2" xr:uid="{0B568844-789D-C748-8E78-B6F61B98CA1B}"/>
     <hyperlink ref="E43" r:id="rId3" xr:uid="{9EE0F42E-8790-A34C-9094-912EF187AA24}"/>
-    <hyperlink ref="E44" r:id="rId4" xr:uid="{D8F20C73-2D3C-1346-984B-28575D1F8F25}"/>
+    <hyperlink ref="E45" r:id="rId4" xr:uid="{D8F20C73-2D3C-1346-984B-28575D1F8F25}"/>
+    <hyperlink ref="E44" r:id="rId5" xr:uid="{E5140E38-A2BE-F743-B187-682A6D818D2E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4043,8 +4067,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D39262A-73A2-9F44-AB0C-854C9E4828A4}">
   <dimension ref="A1:L48"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7:L13"/>
+    <sheetView topLeftCell="E7" workbookViewId="0">
+      <selection activeCell="K35" sqref="K35:K40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -4141,7 +4165,7 @@
       <c r="K5" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="L5" s="14" t="s">
+      <c r="L5" s="16" t="s">
         <v>171</v>
       </c>
     </row>
@@ -4175,7 +4199,7 @@
       <c r="K6" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="L6" s="15"/>
+      <c r="L6" s="17"/>
     </row>
     <row r="7" spans="1:12">
       <c r="A7" s="7">
@@ -4207,7 +4231,7 @@
       <c r="K7" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="L7" s="14" t="s">
+      <c r="L7" s="16" t="s">
         <v>169</v>
       </c>
     </row>
@@ -4241,7 +4265,7 @@
       <c r="K8" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="L8" s="14"/>
+      <c r="L8" s="16"/>
     </row>
     <row r="9" spans="1:12">
       <c r="A9" s="7">
@@ -4273,7 +4297,7 @@
       <c r="K9" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="L9" s="14"/>
+      <c r="L9" s="16"/>
     </row>
     <row r="10" spans="1:12">
       <c r="A10" s="7">
@@ -4305,7 +4329,7 @@
       <c r="K10" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="L10" s="14"/>
+      <c r="L10" s="16"/>
     </row>
     <row r="11" spans="1:12">
       <c r="A11" s="7">
@@ -4337,7 +4361,7 @@
       <c r="K11" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="L11" s="14"/>
+      <c r="L11" s="16"/>
     </row>
     <row r="12" spans="1:12">
       <c r="A12" s="7">
@@ -4369,7 +4393,7 @@
       <c r="K12" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="L12" s="14"/>
+      <c r="L12" s="16"/>
     </row>
     <row r="13" spans="1:12">
       <c r="A13" s="7">
@@ -4401,7 +4425,7 @@
       <c r="K13" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="L13" s="14"/>
+      <c r="L13" s="16"/>
     </row>
     <row r="14" spans="1:12">
       <c r="A14" s="7">
@@ -4433,7 +4457,7 @@
       <c r="K14" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="L14" s="14" t="s">
+      <c r="L14" s="16" t="s">
         <v>170</v>
       </c>
     </row>
@@ -4467,7 +4491,7 @@
       <c r="K15" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="L15" s="15"/>
+      <c r="L15" s="17"/>
     </row>
     <row r="16" spans="1:12">
       <c r="A16" s="7">
@@ -4499,7 +4523,7 @@
       <c r="K16" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="L16" s="15"/>
+      <c r="L16" s="17"/>
     </row>
     <row r="17" spans="1:12">
       <c r="A17" s="7">
@@ -4531,7 +4555,7 @@
       <c r="K17" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="L17" s="15"/>
+      <c r="L17" s="17"/>
     </row>
     <row r="18" spans="1:12">
       <c r="A18" s="7">
@@ -4563,7 +4587,7 @@
       <c r="K18" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="L18" s="15"/>
+      <c r="L18" s="17"/>
     </row>
     <row r="19" spans="1:12">
       <c r="A19" s="7">
@@ -4595,7 +4619,7 @@
       <c r="K19" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="L19" s="15"/>
+      <c r="L19" s="17"/>
     </row>
     <row r="20" spans="1:12">
       <c r="A20" s="7">
@@ -4627,7 +4651,7 @@
       <c r="K20" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="L20" s="15"/>
+      <c r="L20" s="17"/>
     </row>
     <row r="21" spans="1:12">
       <c r="A21" s="7">
@@ -4659,7 +4683,7 @@
       <c r="K21" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="L21" s="15"/>
+      <c r="L21" s="17"/>
     </row>
     <row r="22" spans="1:12">
       <c r="A22" s="7">
@@ -4691,7 +4715,7 @@
       <c r="K22" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="L22" s="15"/>
+      <c r="L22" s="17"/>
     </row>
     <row r="23" spans="1:12">
       <c r="A23" s="7">
@@ -4723,7 +4747,7 @@
       <c r="K23" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="L23" s="14" t="s">
+      <c r="L23" s="16" t="s">
         <v>168</v>
       </c>
     </row>
@@ -4757,7 +4781,7 @@
       <c r="K24" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="L24" s="15"/>
+      <c r="L24" s="17"/>
     </row>
     <row r="25" spans="1:12">
       <c r="A25" s="7">
@@ -4789,7 +4813,7 @@
       <c r="K25" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="L25" s="15"/>
+      <c r="L25" s="17"/>
     </row>
     <row r="26" spans="1:12">
       <c r="A26" s="7">
@@ -4821,7 +4845,7 @@
       <c r="K26" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="L26" s="15"/>
+      <c r="L26" s="17"/>
     </row>
     <row r="27" spans="1:12">
       <c r="A27" s="7">
@@ -4853,7 +4877,7 @@
       <c r="K27" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="L27" s="15"/>
+      <c r="L27" s="17"/>
     </row>
     <row r="28" spans="1:12">
       <c r="A28" s="7">
@@ -4885,7 +4909,7 @@
       <c r="K28" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="L28" s="15"/>
+      <c r="L28" s="17"/>
     </row>
     <row r="29" spans="1:12">
       <c r="A29" s="7">
@@ -4917,7 +4941,7 @@
       <c r="K29" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="L29" s="15"/>
+      <c r="L29" s="17"/>
     </row>
     <row r="30" spans="1:12">
       <c r="A30" s="7">
@@ -4949,7 +4973,7 @@
       <c r="K30" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="L30" s="15"/>
+      <c r="L30" s="17"/>
     </row>
     <row r="31" spans="1:12">
       <c r="A31" s="7">
@@ -4981,7 +5005,7 @@
       <c r="K31" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="L31" s="15"/>
+      <c r="L31" s="17"/>
     </row>
     <row r="32" spans="1:12">
       <c r="A32" s="7">
@@ -5013,7 +5037,7 @@
       <c r="K32" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="L32" s="15"/>
+      <c r="L32" s="17"/>
     </row>
     <row r="33" spans="1:12">
       <c r="A33" s="7">
@@ -5045,7 +5069,7 @@
       <c r="K33" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="L33" s="15"/>
+      <c r="L33" s="17"/>
     </row>
     <row r="34" spans="1:12">
       <c r="A34" s="7">
@@ -5077,7 +5101,7 @@
       <c r="K34" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="L34" s="15"/>
+      <c r="L34" s="17"/>
     </row>
     <row r="35" spans="1:12">
       <c r="A35" s="7">
@@ -5109,7 +5133,7 @@
       <c r="K35" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="L35" s="14" t="s">
+      <c r="L35" s="16" t="s">
         <v>167</v>
       </c>
     </row>
@@ -5143,7 +5167,7 @@
       <c r="K36" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="L36" s="15"/>
+      <c r="L36" s="17"/>
     </row>
     <row r="37" spans="1:12">
       <c r="A37" s="7">
@@ -5175,7 +5199,7 @@
       <c r="K37" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="L37" s="15"/>
+      <c r="L37" s="17"/>
     </row>
     <row r="38" spans="1:12">
       <c r="A38" s="7">
@@ -5207,7 +5231,7 @@
       <c r="K38" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="L38" s="15"/>
+      <c r="L38" s="17"/>
     </row>
     <row r="39" spans="1:12">
       <c r="A39" s="7">
@@ -5239,7 +5263,7 @@
       <c r="K39" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="L39" s="15"/>
+      <c r="L39" s="17"/>
     </row>
     <row r="40" spans="1:12">
       <c r="A40" s="7">
@@ -5271,7 +5295,7 @@
       <c r="K40" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="L40" s="15"/>
+      <c r="L40" s="17"/>
     </row>
     <row r="41" spans="1:12">
       <c r="A41" s="7"/>
@@ -5287,6 +5311,10 @@
       </c>
       <c r="F41" s="7">
         <v>1551000</v>
+      </c>
+      <c r="G41">
+        <f>E41/F41</f>
+        <v>0.84120889748549321</v>
       </c>
     </row>
     <row r="44" spans="1:12">
@@ -5395,8 +5423,8 @@
       <c r="F1" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
     </row>
     <row r="2" spans="1:13">
       <c r="A2" t="s">
@@ -5417,13 +5445,13 @@
       <c r="F2" s="19" t="s">
         <v>86</v>
       </c>
-      <c r="G2" s="18"/>
+      <c r="G2" s="15"/>
     </row>
     <row r="3" spans="1:13" ht="48">
       <c r="A3" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="15" t="s">
         <v>0</v>
       </c>
       <c r="C3" t="s">

</xml_diff>